<commit_message>
final , all works
</commit_message>
<xml_diff>
--- a/demo.xlsx
+++ b/demo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="76">
   <si>
     <t>תעודת זהות</t>
   </si>
@@ -37,6 +37,9 @@
     <t>תאריכים א</t>
   </si>
   <si>
+    <t>איש קשר אחראי א</t>
+  </si>
+  <si>
     <t>התנסות ב</t>
   </si>
   <si>
@@ -46,6 +49,9 @@
     <t>תאריכים ב</t>
   </si>
   <si>
+    <t>איש קשר אחראי ב</t>
+  </si>
+  <si>
     <t>התנסות ג</t>
   </si>
   <si>
@@ -55,6 +61,9 @@
     <t>תאריכים ג</t>
   </si>
   <si>
+    <t>איש קשר אחראי ג</t>
+  </si>
+  <si>
     <t>התנסות ד</t>
   </si>
   <si>
@@ -64,6 +73,9 @@
     <t>תאריכים ד</t>
   </si>
   <si>
+    <t>איש קשר אחראי ד</t>
+  </si>
+  <si>
     <t>התנסות ה</t>
   </si>
   <si>
@@ -73,6 +85,9 @@
     <t>תאריכים ה</t>
   </si>
   <si>
+    <t>איש קשר אחראי ה</t>
+  </si>
+  <si>
     <t>הערות</t>
   </si>
   <si>
@@ -145,36 +160,12 @@
     <t>רחלי ברוכים</t>
   </si>
   <si>
-    <t>הדר אבגי</t>
-  </si>
-  <si>
-    <t>שובל אגשם</t>
-  </si>
-  <si>
-    <t>מאיה אדרי</t>
-  </si>
-  <si>
-    <t>ספיר אהרן</t>
-  </si>
-  <si>
-    <t>יעל אורגלר</t>
-  </si>
-  <si>
-    <t>אודיה אטיאס</t>
-  </si>
-  <si>
-    <t>נתנאל אלגוזי</t>
-  </si>
-  <si>
     <t>ב</t>
   </si>
   <si>
     <t>ג</t>
   </si>
   <si>
-    <t>ד</t>
-  </si>
-  <si>
     <t>אריאל</t>
   </si>
   <si>
@@ -187,49 +178,61 @@
     <t>כפר סבא</t>
   </si>
   <si>
+    <t>ס.המבוגר - פנימית</t>
+  </si>
+  <si>
     <t>ס.המבוגר - כירורגית</t>
   </si>
   <si>
     <t>טראומה מלרד - מיון</t>
   </si>
   <si>
+    <t>בלינסון</t>
+  </si>
+  <si>
     <t>מאיר</t>
   </si>
   <si>
+    <t>שניידר</t>
+  </si>
+  <si>
     <t>שערי צדק</t>
   </si>
   <si>
     <t>27.2.22-13.4.22</t>
   </si>
   <si>
-    <t>11.7.21-29.7.21</t>
-  </si>
-  <si>
-    <t>1.8.21-19.8.21</t>
-  </si>
-  <si>
-    <t>ס.המבוגר - פנימית</t>
+    <t>22.8.21-14.9.21</t>
+  </si>
+  <si>
+    <t>10.10.21-3.11.21</t>
+  </si>
+  <si>
+    <t>5.12.21-30.12.21</t>
+  </si>
+  <si>
+    <t>7.11.21-2.12.21</t>
+  </si>
+  <si>
+    <t>ישראל;0542568946;israel@gamil.com</t>
+  </si>
+  <si>
+    <t>מוטי;0541234512;Moti@gamil.com</t>
   </si>
   <si>
     <t>ס.ילד - ילדים</t>
   </si>
   <si>
-    <t>בלינסון</t>
-  </si>
-  <si>
     <t>24.4.22-8.6.22</t>
   </si>
   <si>
-    <t>7.11.21-2.12.21</t>
-  </si>
-  <si>
-    <t>10.10.21-3.11.21</t>
+    <t>27.2.22-24.3.22</t>
+  </si>
+  <si>
+    <t>27.3.22-28.4.22</t>
   </si>
   <si>
     <t>ס.אישה - ס.אישה</t>
-  </si>
-  <si>
-    <t>שניידר</t>
   </si>
   <si>
     <t>הסטודנט שובץ בהכל</t>
@@ -306,7 +309,68 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB73A3A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF23C26F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF438FFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD83B01"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF72FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -596,13 +660,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T31"/>
+  <dimension ref="A1:Y24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="3.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="33.7109375" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" customWidth="1"/>
+    <col min="12" max="12" width="33.7109375" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="16.7109375" customWidth="1"/>
+    <col min="16" max="16" width="33.7109375" customWidth="1"/>
+    <col min="17" max="17" width="8.7109375" customWidth="1"/>
+    <col min="18" max="18" width="11.7109375" customWidth="1"/>
+    <col min="19" max="19" width="9.7109375" customWidth="1"/>
+    <col min="20" max="20" width="15.7109375" customWidth="1"/>
+    <col min="21" max="21" width="8.7109375" customWidth="1"/>
+    <col min="22" max="22" width="11.7109375" customWidth="1"/>
+    <col min="23" max="23" width="9.7109375" customWidth="1"/>
+    <col min="24" max="24" width="15.7109375" customWidth="1"/>
+    <col min="25" max="25" width="41.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -663,977 +754,1104 @@
       <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:20">
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25">
       <c r="A2">
         <v>206837353</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
         <v>50</v>
       </c>
-      <c r="D2" t="s">
-        <v>53</v>
-      </c>
       <c r="E2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" t="s">
         <v>57</v>
-      </c>
-      <c r="F2" t="s">
-        <v>59</v>
       </c>
       <c r="G2" t="s">
         <v>61</v>
       </c>
       <c r="H2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" t="s">
         <v>59</v>
       </c>
-      <c r="J2" t="s">
-        <v>67</v>
-      </c>
-      <c r="T2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20">
+      <c r="K2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25">
       <c r="A3">
         <v>315843607</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" t="s">
         <v>54</v>
       </c>
-      <c r="T3" t="s">
+      <c r="F3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:25">
       <c r="A4">
         <v>209149889</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" t="s">
         <v>57</v>
-      </c>
-      <c r="F4" t="s">
-        <v>59</v>
       </c>
       <c r="G4" t="s">
         <v>61</v>
       </c>
       <c r="H4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J4" t="s">
         <v>59</v>
       </c>
-      <c r="J4" t="s">
-        <v>67</v>
-      </c>
-      <c r="T4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20">
+      <c r="K4" t="s">
+        <v>69</v>
+      </c>
+      <c r="L4" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25">
       <c r="A5">
         <v>322639030</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" t="s">
         <v>57</v>
-      </c>
-      <c r="F5" t="s">
-        <v>59</v>
       </c>
       <c r="G5" t="s">
         <v>61</v>
       </c>
       <c r="H5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J5" t="s">
         <v>59</v>
       </c>
-      <c r="J5" t="s">
-        <v>67</v>
-      </c>
-      <c r="T5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20">
+      <c r="K5" t="s">
+        <v>69</v>
+      </c>
+      <c r="L5" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25">
       <c r="A6">
         <v>314956517</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" t="s">
         <v>57</v>
-      </c>
-      <c r="F6" t="s">
-        <v>59</v>
       </c>
       <c r="G6" t="s">
         <v>61</v>
       </c>
       <c r="H6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I6" t="s">
+        <v>55</v>
+      </c>
+      <c r="J6" t="s">
         <v>59</v>
       </c>
-      <c r="J6" t="s">
-        <v>67</v>
-      </c>
-      <c r="T6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20">
+      <c r="K6" t="s">
+        <v>69</v>
+      </c>
+      <c r="L6" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25">
       <c r="A7">
         <v>206531881</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" t="s">
         <v>54</v>
       </c>
-      <c r="T7" t="s">
+      <c r="F7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H7" t="s">
+        <v>66</v>
+      </c>
+      <c r="I7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J7" t="s">
+        <v>59</v>
+      </c>
+      <c r="K7" t="s">
+        <v>69</v>
+      </c>
+      <c r="L7" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y7" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:25">
       <c r="A8">
         <v>205376627</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" t="s">
         <v>55</v>
       </c>
-      <c r="E8" t="s">
-        <v>57</v>
-      </c>
       <c r="F8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G8" t="s">
         <v>61</v>
       </c>
       <c r="H8" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I8" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="J8" t="s">
-        <v>67</v>
-      </c>
-      <c r="T8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20">
+        <v>58</v>
+      </c>
+      <c r="K8" t="s">
+        <v>69</v>
+      </c>
+      <c r="L8" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25">
       <c r="A9">
         <v>314713603</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" t="s">
         <v>55</v>
       </c>
-      <c r="E9" t="s">
-        <v>57</v>
-      </c>
       <c r="F9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G9" t="s">
         <v>61</v>
       </c>
       <c r="H9" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I9" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="J9" t="s">
-        <v>67</v>
-      </c>
-      <c r="T9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20">
+        <v>58</v>
+      </c>
+      <c r="K9" t="s">
+        <v>69</v>
+      </c>
+      <c r="L9" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25">
       <c r="A10">
         <v>318960150</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G10" t="s">
         <v>61</v>
       </c>
       <c r="H10" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="J10" t="s">
-        <v>67</v>
-      </c>
-      <c r="T10" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20">
+        <v>58</v>
+      </c>
+      <c r="K10" t="s">
+        <v>69</v>
+      </c>
+      <c r="L10" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25">
       <c r="A11">
         <v>206360562</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D11" t="s">
-        <v>54</v>
-      </c>
-      <c r="T11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20">
+        <v>51</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25">
       <c r="A12">
         <v>211542063</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" t="s">
         <v>55</v>
       </c>
-      <c r="E12" t="s">
-        <v>57</v>
-      </c>
       <c r="F12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G12" t="s">
         <v>61</v>
       </c>
       <c r="H12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I12" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="J12" t="s">
-        <v>67</v>
-      </c>
-      <c r="T12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20">
+        <v>58</v>
+      </c>
+      <c r="K12" t="s">
+        <v>69</v>
+      </c>
+      <c r="L12" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25">
       <c r="A13">
         <v>208284471</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" t="s">
         <v>55</v>
       </c>
-      <c r="E13" t="s">
-        <v>57</v>
-      </c>
       <c r="F13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G13" t="s">
         <v>61</v>
       </c>
       <c r="H13" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I13" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="J13" t="s">
-        <v>67</v>
-      </c>
-      <c r="T13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20">
+        <v>58</v>
+      </c>
+      <c r="K13" t="s">
+        <v>69</v>
+      </c>
+      <c r="L13" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25">
       <c r="A14">
         <v>209371384</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" t="s">
         <v>56</v>
       </c>
-      <c r="E14" t="s">
-        <v>58</v>
-      </c>
       <c r="F14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G14" t="s">
         <v>62</v>
       </c>
       <c r="H14" t="s">
+        <v>66</v>
+      </c>
+      <c r="I14" t="s">
+        <v>68</v>
+      </c>
+      <c r="J14" t="s">
+        <v>59</v>
+      </c>
+      <c r="K14" t="s">
+        <v>64</v>
+      </c>
+      <c r="L14" t="s">
+        <v>67</v>
+      </c>
+      <c r="M14" t="s">
+        <v>72</v>
+      </c>
+      <c r="N14" t="s">
+        <v>58</v>
+      </c>
+      <c r="O14" t="s">
         <v>65</v>
       </c>
-      <c r="I14" t="s">
-        <v>66</v>
-      </c>
-      <c r="J14" t="s">
-        <v>68</v>
-      </c>
-      <c r="K14" t="s">
-        <v>70</v>
-      </c>
-      <c r="L14" t="s">
-        <v>71</v>
-      </c>
-      <c r="M14" t="s">
-        <v>69</v>
-      </c>
-      <c r="T14" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20">
+      <c r="P14" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25">
       <c r="A15">
         <v>209007186</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" t="s">
         <v>51</v>
       </c>
-      <c r="D15" t="s">
-        <v>54</v>
-      </c>
       <c r="E15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I15" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="J15" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="K15" t="s">
+        <v>64</v>
+      </c>
+      <c r="L15" t="s">
+        <v>67</v>
+      </c>
+      <c r="M15" t="s">
+        <v>72</v>
+      </c>
+      <c r="N15" t="s">
+        <v>57</v>
+      </c>
+      <c r="O15" t="s">
         <v>70</v>
       </c>
-      <c r="L15" t="s">
-        <v>71</v>
-      </c>
-      <c r="M15" t="s">
-        <v>69</v>
-      </c>
-      <c r="T15" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20">
+      <c r="P15" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25">
       <c r="A16">
         <v>315828624</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D16" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G16" t="s">
         <v>62</v>
       </c>
       <c r="H16" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I16" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="J16" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="K16" t="s">
+        <v>64</v>
+      </c>
+      <c r="L16" t="s">
+        <v>67</v>
+      </c>
+      <c r="M16" t="s">
+        <v>72</v>
+      </c>
+      <c r="N16" t="s">
+        <v>57</v>
+      </c>
+      <c r="O16" t="s">
         <v>70</v>
       </c>
-      <c r="L16" t="s">
-        <v>71</v>
-      </c>
-      <c r="M16" t="s">
-        <v>69</v>
-      </c>
-      <c r="T16" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20">
+      <c r="P16" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25">
       <c r="A17">
         <v>318124062</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D17" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G17" t="s">
         <v>62</v>
       </c>
       <c r="H17" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I17" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="J17" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="K17" t="s">
+        <v>64</v>
+      </c>
+      <c r="L17" t="s">
+        <v>67</v>
+      </c>
+      <c r="M17" t="s">
+        <v>72</v>
+      </c>
+      <c r="N17" t="s">
+        <v>57</v>
+      </c>
+      <c r="O17" t="s">
         <v>70</v>
       </c>
-      <c r="L17" t="s">
-        <v>71</v>
-      </c>
-      <c r="M17" t="s">
-        <v>69</v>
-      </c>
-      <c r="T17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20">
+      <c r="P17" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25">
       <c r="A18">
         <v>208115428</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" t="s">
         <v>56</v>
-      </c>
-      <c r="E18" t="s">
-        <v>58</v>
       </c>
       <c r="F18" t="s">
         <v>59</v>
       </c>
       <c r="G18" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H18" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="I18" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J18" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="K18" t="s">
         <v>70</v>
       </c>
       <c r="L18" t="s">
+        <v>66</v>
+      </c>
+      <c r="M18" t="s">
+        <v>72</v>
+      </c>
+      <c r="N18" t="s">
+        <v>59</v>
+      </c>
+      <c r="O18" t="s">
         <v>71</v>
       </c>
-      <c r="M18" t="s">
-        <v>69</v>
-      </c>
-      <c r="T18" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20">
+      <c r="P18" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25">
       <c r="A19">
         <v>206788853</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" t="s">
         <v>51</v>
       </c>
-      <c r="D19" t="s">
-        <v>54</v>
-      </c>
       <c r="E19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G19" t="s">
         <v>63</v>
       </c>
       <c r="H19" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="I19" t="s">
+        <v>68</v>
+      </c>
+      <c r="J19" t="s">
         <v>60</v>
       </c>
-      <c r="J19" t="s">
-        <v>69</v>
-      </c>
       <c r="K19" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="L19" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="M19" t="s">
-        <v>69</v>
-      </c>
-      <c r="T19" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20">
+        <v>72</v>
+      </c>
+      <c r="N19" t="s">
+        <v>60</v>
+      </c>
+      <c r="O19" t="s">
+        <v>64</v>
+      </c>
+      <c r="P19" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25">
       <c r="A20">
         <v>318334026</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D20" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F20" t="s">
         <v>59</v>
       </c>
       <c r="G20" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H20" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="I20" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="J20" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="K20" t="s">
         <v>70</v>
       </c>
       <c r="L20" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="M20" t="s">
-        <v>69</v>
-      </c>
-      <c r="T20" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20">
+        <v>72</v>
+      </c>
+      <c r="N20" t="s">
+        <v>60</v>
+      </c>
+      <c r="O20" t="s">
+        <v>64</v>
+      </c>
+      <c r="P20" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25">
       <c r="A21">
         <v>207402900</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D21" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E21" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F21" t="s">
         <v>59</v>
       </c>
       <c r="G21" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H21" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="I21" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="J21" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="K21" t="s">
         <v>70</v>
       </c>
       <c r="L21" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="M21" t="s">
-        <v>69</v>
-      </c>
-      <c r="T21" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20">
+        <v>72</v>
+      </c>
+      <c r="N21" t="s">
+        <v>60</v>
+      </c>
+      <c r="O21" t="s">
+        <v>64</v>
+      </c>
+      <c r="P21" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25">
       <c r="A22">
         <v>207726332</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C22" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D22" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" t="s">
         <v>56</v>
-      </c>
-      <c r="E22" t="s">
-        <v>58</v>
       </c>
       <c r="F22" t="s">
         <v>59</v>
       </c>
       <c r="G22" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H22" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="I22" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J22" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="K22" t="s">
         <v>70</v>
       </c>
       <c r="L22" t="s">
+        <v>66</v>
+      </c>
+      <c r="M22" t="s">
+        <v>72</v>
+      </c>
+      <c r="N22" t="s">
+        <v>59</v>
+      </c>
+      <c r="O22" t="s">
         <v>71</v>
       </c>
-      <c r="M22" t="s">
-        <v>69</v>
-      </c>
-      <c r="T22" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20">
+      <c r="P22" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25">
       <c r="A23">
         <v>208825745</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" t="s">
         <v>51</v>
       </c>
-      <c r="D23" t="s">
-        <v>54</v>
-      </c>
       <c r="E23" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F23" t="s">
         <v>60</v>
       </c>
       <c r="G23" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="I23" t="s">
+        <v>68</v>
+      </c>
+      <c r="J23" t="s">
         <v>60</v>
       </c>
-      <c r="J23" t="s">
-        <v>69</v>
-      </c>
       <c r="K23" t="s">
+        <v>71</v>
+      </c>
+      <c r="L23" t="s">
+        <v>67</v>
+      </c>
+      <c r="M23" t="s">
+        <v>72</v>
+      </c>
+      <c r="N23" t="s">
+        <v>57</v>
+      </c>
+      <c r="O23" t="s">
         <v>70</v>
       </c>
-      <c r="L23" t="s">
-        <v>71</v>
-      </c>
-      <c r="M23" t="s">
-        <v>69</v>
-      </c>
-      <c r="T23" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20">
+      <c r="P23" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25">
       <c r="A24">
         <v>205419864</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C24" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D24" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E24" t="s">
+        <v>56</v>
+      </c>
+      <c r="F24" t="s">
         <v>58</v>
       </c>
-      <c r="F24" t="s">
-        <v>59</v>
-      </c>
       <c r="G24" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="H24" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I24" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="J24" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="K24" t="s">
         <v>70</v>
       </c>
       <c r="L24" t="s">
+        <v>66</v>
+      </c>
+      <c r="M24" t="s">
+        <v>72</v>
+      </c>
+      <c r="N24" t="s">
+        <v>59</v>
+      </c>
+      <c r="O24" t="s">
         <v>71</v>
       </c>
-      <c r="M24" t="s">
-        <v>69</v>
-      </c>
-      <c r="T24" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20">
-      <c r="A25">
-        <v>208753103</v>
-      </c>
-      <c r="B25" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" t="s">
-        <v>52</v>
-      </c>
-      <c r="D25" t="s">
-        <v>55</v>
-      </c>
-      <c r="T25" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20">
-      <c r="A26">
-        <v>318515145</v>
-      </c>
-      <c r="B26" t="s">
-        <v>44</v>
-      </c>
-      <c r="C26" t="s">
-        <v>52</v>
-      </c>
-      <c r="D26" t="s">
-        <v>56</v>
-      </c>
-      <c r="T26" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20">
-      <c r="A27">
-        <v>206957805</v>
-      </c>
-      <c r="B27" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27" t="s">
-        <v>52</v>
-      </c>
-      <c r="D27" t="s">
-        <v>54</v>
-      </c>
-      <c r="T27" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20">
-      <c r="A28">
-        <v>311382337</v>
-      </c>
-      <c r="B28" t="s">
-        <v>46</v>
-      </c>
-      <c r="C28" t="s">
-        <v>52</v>
-      </c>
-      <c r="D28" t="s">
-        <v>55</v>
-      </c>
-      <c r="T28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20">
-      <c r="A29">
-        <v>318811395</v>
-      </c>
-      <c r="B29" t="s">
-        <v>47</v>
-      </c>
-      <c r="C29" t="s">
-        <v>52</v>
-      </c>
-      <c r="D29" t="s">
-        <v>56</v>
-      </c>
-      <c r="T29" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20">
-      <c r="A30">
-        <v>206948317</v>
-      </c>
-      <c r="B30" t="s">
-        <v>48</v>
-      </c>
-      <c r="C30" t="s">
-        <v>52</v>
-      </c>
-      <c r="D30" t="s">
-        <v>56</v>
-      </c>
-      <c r="T30" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20">
-      <c r="A31">
-        <v>307923284</v>
-      </c>
-      <c r="B31" t="s">
-        <v>49</v>
-      </c>
-      <c r="C31" t="s">
-        <v>52</v>
-      </c>
-      <c r="D31" t="s">
-        <v>55</v>
-      </c>
-      <c r="T31" t="s">
-        <v>73</v>
+      <c r="P24" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E1:H1">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I1:L1">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M1:P1">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q1:T1">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U1:X1">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y2:Y24">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"בעיה - לא שובץ בכלום!"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>